<commit_message>
Projeto RPG HROADS feito
</commit_message>
<xml_diff>
--- a/planejamento/cronograma/2021-1S-2D-cronograma.xlsx
+++ b/planejamento/cronograma/2021-1S-2D-cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saulo.santos\Downloads\SENAI\CT\2021-1S-2D\senai-dev-1s2021-alunos\planejamento\cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36C799E-8721-402D-A9FF-F8F647FF1EFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4137652-F8AA-4FC0-A040-ECB28D90C775}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="100">
   <si>
     <t>3. Desenvolver interfaces web utilizando frameworks</t>
   </si>
@@ -324,6 +324,9 @@
   </si>
   <si>
     <t>Roman</t>
+  </si>
+  <si>
+    <t>de aula</t>
   </si>
 </sst>
 </file>
@@ -993,7 +996,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1144,7 +1147,6 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="19" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1187,28 +1189,15 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1228,6 +1217,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1611,7 +1609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B41537EB-D492-4302-88EF-5E854D108BA5}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -1626,9 +1624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A77"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2016,8 +2012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:FD55"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="X3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
@@ -2054,117 +2050,117 @@
   <sheetData>
     <row r="1" spans="1:160" x14ac:dyDescent="0.3">
       <c r="A1" s="95"/>
-      <c r="B1" s="147" t="s">
+      <c r="B1" s="157" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="148"/>
-      <c r="D1" s="148"/>
-      <c r="E1" s="148"/>
-      <c r="F1" s="148"/>
-      <c r="G1" s="148"/>
-      <c r="H1" s="148"/>
-      <c r="I1" s="148"/>
-      <c r="J1" s="148"/>
-      <c r="K1" s="148"/>
-      <c r="L1" s="148"/>
-      <c r="M1" s="148"/>
-      <c r="N1" s="148"/>
-      <c r="O1" s="148"/>
-      <c r="P1" s="149"/>
-      <c r="Q1" s="150" t="s">
+      <c r="C1" s="158"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="158"/>
+      <c r="G1" s="158"/>
+      <c r="H1" s="158"/>
+      <c r="I1" s="158"/>
+      <c r="J1" s="158"/>
+      <c r="K1" s="158"/>
+      <c r="L1" s="158"/>
+      <c r="M1" s="158"/>
+      <c r="N1" s="158"/>
+      <c r="O1" s="158"/>
+      <c r="P1" s="158"/>
+      <c r="Q1" s="158"/>
+      <c r="R1" s="159"/>
+      <c r="S1" s="144" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="151"/>
-      <c r="S1" s="151"/>
-      <c r="T1" s="151"/>
-      <c r="U1" s="151"/>
-      <c r="V1" s="151"/>
-      <c r="W1" s="151"/>
-      <c r="X1" s="151"/>
-      <c r="Y1" s="151"/>
-      <c r="Z1" s="151"/>
-      <c r="AA1" s="151"/>
-      <c r="AB1" s="151"/>
-      <c r="AC1" s="151"/>
-      <c r="AD1" s="151"/>
-      <c r="AE1" s="151"/>
-      <c r="AF1" s="151"/>
-      <c r="AG1" s="151"/>
-      <c r="AH1" s="151"/>
-      <c r="AI1" s="151"/>
-      <c r="AJ1" s="151"/>
-      <c r="AK1" s="151"/>
-      <c r="AL1" s="151"/>
-      <c r="AM1" s="151"/>
-      <c r="AN1" s="151"/>
-      <c r="AO1" s="152"/>
-      <c r="AP1" s="156" t="s">
+      <c r="T1" s="145"/>
+      <c r="U1" s="145"/>
+      <c r="V1" s="145"/>
+      <c r="W1" s="145"/>
+      <c r="X1" s="145"/>
+      <c r="Y1" s="145"/>
+      <c r="Z1" s="145"/>
+      <c r="AA1" s="145"/>
+      <c r="AB1" s="145"/>
+      <c r="AC1" s="145"/>
+      <c r="AD1" s="145"/>
+      <c r="AE1" s="145"/>
+      <c r="AF1" s="145"/>
+      <c r="AG1" s="145"/>
+      <c r="AH1" s="145"/>
+      <c r="AI1" s="145"/>
+      <c r="AJ1" s="145"/>
+      <c r="AK1" s="145"/>
+      <c r="AL1" s="145"/>
+      <c r="AM1" s="145"/>
+      <c r="AN1" s="145"/>
+      <c r="AO1" s="146"/>
+      <c r="AP1" s="154" t="s">
         <v>50</v>
       </c>
-      <c r="AQ1" s="157"/>
-      <c r="AR1" s="157"/>
-      <c r="AS1" s="158"/>
-      <c r="AT1" s="157" t="s">
+      <c r="AQ1" s="155"/>
+      <c r="AR1" s="155"/>
+      <c r="AS1" s="156"/>
+      <c r="AT1" s="155" t="s">
         <v>51</v>
       </c>
-      <c r="AU1" s="157"/>
-      <c r="AV1" s="157"/>
-      <c r="AW1" s="157"/>
-      <c r="AX1" s="157"/>
-      <c r="AY1" s="157"/>
-      <c r="AZ1" s="157"/>
-      <c r="BA1" s="157"/>
-      <c r="BB1" s="157"/>
-      <c r="BC1" s="157"/>
-      <c r="BD1" s="157"/>
-      <c r="BE1" s="157"/>
-      <c r="BF1" s="157"/>
-      <c r="BG1" s="157"/>
-      <c r="BH1" s="157"/>
-      <c r="BI1" s="157"/>
-      <c r="BJ1" s="157"/>
-      <c r="BK1" s="157"/>
-      <c r="BL1" s="157"/>
-      <c r="BM1" s="157"/>
-      <c r="BN1" s="158"/>
-      <c r="BO1" s="153" t="s">
+      <c r="AU1" s="155"/>
+      <c r="AV1" s="155"/>
+      <c r="AW1" s="155"/>
+      <c r="AX1" s="155"/>
+      <c r="AY1" s="155"/>
+      <c r="AZ1" s="155"/>
+      <c r="BA1" s="155"/>
+      <c r="BB1" s="155"/>
+      <c r="BC1" s="155"/>
+      <c r="BD1" s="155"/>
+      <c r="BE1" s="155"/>
+      <c r="BF1" s="155"/>
+      <c r="BG1" s="155"/>
+      <c r="BH1" s="155"/>
+      <c r="BI1" s="155"/>
+      <c r="BJ1" s="155"/>
+      <c r="BK1" s="155"/>
+      <c r="BL1" s="155"/>
+      <c r="BM1" s="155"/>
+      <c r="BN1" s="156"/>
+      <c r="BO1" s="151" t="s">
         <v>52</v>
       </c>
-      <c r="BP1" s="154"/>
-      <c r="BQ1" s="154"/>
-      <c r="BR1" s="154"/>
-      <c r="BS1" s="154"/>
-      <c r="BT1" s="154"/>
-      <c r="BU1" s="154"/>
-      <c r="BV1" s="154"/>
-      <c r="BW1" s="154"/>
-      <c r="BX1" s="154"/>
-      <c r="BY1" s="154"/>
-      <c r="BZ1" s="154"/>
-      <c r="CA1" s="154"/>
-      <c r="CB1" s="154"/>
-      <c r="CC1" s="154"/>
-      <c r="CD1" s="154"/>
-      <c r="CE1" s="154"/>
-      <c r="CF1" s="154"/>
-      <c r="CG1" s="154"/>
-      <c r="CH1" s="155"/>
-      <c r="CI1" s="145" t="s">
+      <c r="BP1" s="152"/>
+      <c r="BQ1" s="152"/>
+      <c r="BR1" s="152"/>
+      <c r="BS1" s="152"/>
+      <c r="BT1" s="152"/>
+      <c r="BU1" s="152"/>
+      <c r="BV1" s="152"/>
+      <c r="BW1" s="152"/>
+      <c r="BX1" s="152"/>
+      <c r="BY1" s="152"/>
+      <c r="BZ1" s="152"/>
+      <c r="CA1" s="152"/>
+      <c r="CB1" s="152"/>
+      <c r="CC1" s="152"/>
+      <c r="CD1" s="152"/>
+      <c r="CE1" s="152"/>
+      <c r="CF1" s="152"/>
+      <c r="CG1" s="152"/>
+      <c r="CH1" s="153"/>
+      <c r="CI1" s="149" t="s">
         <v>78</v>
       </c>
-      <c r="CJ1" s="145"/>
-      <c r="CK1" s="145"/>
-      <c r="CL1" s="145"/>
-      <c r="CM1" s="145"/>
-      <c r="CN1" s="145"/>
-      <c r="CO1" s="145"/>
-      <c r="CP1" s="145"/>
-      <c r="CQ1" s="145"/>
-      <c r="CR1" s="145"/>
-      <c r="CS1" s="145"/>
-      <c r="CT1" s="145"/>
-      <c r="CU1" s="145"/>
-      <c r="CV1" s="146"/>
+      <c r="CJ1" s="149"/>
+      <c r="CK1" s="149"/>
+      <c r="CL1" s="149"/>
+      <c r="CM1" s="149"/>
+      <c r="CN1" s="149"/>
+      <c r="CO1" s="149"/>
+      <c r="CP1" s="149"/>
+      <c r="CQ1" s="149"/>
+      <c r="CR1" s="149"/>
+      <c r="CS1" s="149"/>
+      <c r="CT1" s="149"/>
+      <c r="CU1" s="149"/>
+      <c r="CV1" s="150"/>
     </row>
     <row r="2" spans="1:160" s="39" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="80" t="s">
@@ -2212,13 +2208,13 @@
       <c r="O2" s="71">
         <v>44264</v>
       </c>
-      <c r="P2" s="71">
+      <c r="P2" s="147">
         <v>44265</v>
       </c>
-      <c r="Q2" s="112">
+      <c r="Q2" s="147">
         <v>44266</v>
       </c>
-      <c r="R2" s="72">
+      <c r="R2" s="148">
         <v>44267</v>
       </c>
       <c r="S2" s="72">
@@ -2287,7 +2283,7 @@
       <c r="AN2" s="72">
         <v>44300</v>
       </c>
-      <c r="AO2" s="118">
+      <c r="AO2" s="117">
         <v>44301</v>
       </c>
       <c r="AP2" s="74">
@@ -2299,10 +2295,10 @@
       <c r="AR2" s="74">
         <v>44306</v>
       </c>
-      <c r="AS2" s="120">
+      <c r="AS2" s="119">
         <v>44308</v>
       </c>
-      <c r="AT2" s="124">
+      <c r="AT2" s="123">
         <v>44309</v>
       </c>
       <c r="AU2" s="74">
@@ -2362,67 +2358,67 @@
       <c r="BM2" s="74">
         <v>44336</v>
       </c>
-      <c r="BN2" s="120">
+      <c r="BN2" s="119">
         <v>44337</v>
       </c>
-      <c r="BO2" s="116">
+      <c r="BO2" s="115">
         <v>44340</v>
       </c>
-      <c r="BP2" s="116">
+      <c r="BP2" s="115">
         <v>44341</v>
       </c>
-      <c r="BQ2" s="116">
+      <c r="BQ2" s="115">
         <v>44342</v>
       </c>
-      <c r="BR2" s="116">
+      <c r="BR2" s="115">
         <v>44343</v>
       </c>
-      <c r="BS2" s="116">
+      <c r="BS2" s="115">
         <v>44344</v>
       </c>
-      <c r="BT2" s="116">
+      <c r="BT2" s="115">
         <v>44347</v>
       </c>
-      <c r="BU2" s="116">
+      <c r="BU2" s="115">
         <v>44348</v>
       </c>
-      <c r="BV2" s="116">
+      <c r="BV2" s="115">
         <v>44349</v>
       </c>
-      <c r="BW2" s="116">
+      <c r="BW2" s="115">
         <v>44354</v>
       </c>
-      <c r="BX2" s="116">
+      <c r="BX2" s="115">
         <v>44355</v>
       </c>
-      <c r="BY2" s="116">
+      <c r="BY2" s="115">
         <v>44356</v>
       </c>
-      <c r="BZ2" s="116">
+      <c r="BZ2" s="115">
         <v>44357</v>
       </c>
-      <c r="CA2" s="116">
+      <c r="CA2" s="115">
         <v>44358</v>
       </c>
-      <c r="CB2" s="116">
+      <c r="CB2" s="115">
         <v>44361</v>
       </c>
-      <c r="CC2" s="116">
+      <c r="CC2" s="115">
         <v>44362</v>
       </c>
-      <c r="CD2" s="116">
+      <c r="CD2" s="115">
         <v>44363</v>
       </c>
-      <c r="CE2" s="116">
+      <c r="CE2" s="115">
         <v>44364</v>
       </c>
-      <c r="CF2" s="116">
+      <c r="CF2" s="115">
         <v>44365</v>
       </c>
-      <c r="CG2" s="116">
+      <c r="CG2" s="115">
         <v>44368</v>
       </c>
-      <c r="CH2" s="121">
+      <c r="CH2" s="120">
         <v>44369</v>
       </c>
       <c r="CI2" s="75">
@@ -2464,7 +2460,7 @@
       <c r="CU2" s="75">
         <v>44389</v>
       </c>
-      <c r="CV2" s="117">
+      <c r="CV2" s="116">
         <v>44390</v>
       </c>
       <c r="CW2"/>
@@ -2539,12 +2535,13 @@
       <c r="F3" s="22"/>
       <c r="H3" s="41"/>
       <c r="I3" s="22"/>
-      <c r="J3" s="41"/>
+      <c r="J3" s="22"/>
       <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
       <c r="N3" s="22"/>
       <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="22"/>
@@ -2697,13 +2694,13 @@
       <c r="B4" s="43"/>
       <c r="C4" s="111"/>
       <c r="H4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="L4" s="113" t="s">
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="O4" s="112" t="s">
         <v>79</v>
       </c>
-      <c r="N4" s="111"/>
-      <c r="O4" s="111"/>
-      <c r="P4" s="111"/>
+      <c r="Q4" s="111"/>
+      <c r="R4" s="111"/>
       <c r="CV4" s="44"/>
       <c r="CW4"/>
       <c r="CX4"/>
@@ -2773,8 +2770,9 @@
       <c r="B5" s="43"/>
       <c r="C5" s="111"/>
       <c r="H5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="L5" s="115"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="O5" s="114"/>
       <c r="CV5" s="44"/>
       <c r="CW5"/>
       <c r="CX5"/>
@@ -2844,13 +2842,18 @@
       <c r="B6" s="45"/>
       <c r="D6" s="111"/>
       <c r="E6" s="111"/>
-      <c r="I6" s="113" t="s">
+      <c r="I6" s="112" t="s">
         <v>83</v>
       </c>
-      <c r="L6" s="111"/>
-      <c r="N6" s="111"/>
+      <c r="J6" s="112" t="s">
+        <v>83</v>
+      </c>
+      <c r="K6" s="112" t="s">
+        <v>83</v>
+      </c>
       <c r="O6" s="111"/>
-      <c r="P6" s="111"/>
+      <c r="Q6" s="111"/>
+      <c r="R6" s="111"/>
       <c r="CV6" s="44"/>
       <c r="CW6"/>
       <c r="CX6"/>
@@ -2920,10 +2923,11 @@
       <c r="B7" s="45"/>
       <c r="F7" s="111"/>
       <c r="I7" s="111"/>
-      <c r="L7" s="111"/>
-      <c r="N7" s="111"/>
+      <c r="J7" s="111"/>
+      <c r="K7" s="111"/>
       <c r="O7" s="111"/>
-      <c r="P7" s="111"/>
+      <c r="Q7" s="111"/>
+      <c r="R7" s="111"/>
       <c r="CV7" s="44"/>
       <c r="CW7"/>
       <c r="CX7"/>
@@ -2993,10 +2997,11 @@
       <c r="B8" s="45"/>
       <c r="F8" s="111"/>
       <c r="I8" s="111"/>
-      <c r="L8" s="111"/>
-      <c r="N8" s="111"/>
+      <c r="J8" s="111"/>
+      <c r="K8" s="111"/>
       <c r="O8" s="111"/>
-      <c r="P8" s="111"/>
+      <c r="Q8" s="111"/>
+      <c r="R8" s="111"/>
       <c r="CV8" s="44"/>
       <c r="CW8"/>
       <c r="CX8"/>
@@ -3068,13 +3073,14 @@
       <c r="E9" s="111"/>
       <c r="F9" s="111"/>
       <c r="I9" s="111"/>
-      <c r="L9" s="111"/>
-      <c r="M9" s="113" t="s">
+      <c r="J9" s="111"/>
+      <c r="K9" s="111"/>
+      <c r="O9" s="111"/>
+      <c r="P9" s="112" t="s">
         <v>79</v>
       </c>
-      <c r="N9" s="111"/>
-      <c r="O9" s="111"/>
-      <c r="P9" s="111"/>
+      <c r="Q9" s="111"/>
+      <c r="R9" s="111"/>
       <c r="CV9" s="44"/>
       <c r="CW9"/>
       <c r="CX9"/>
@@ -3144,10 +3150,11 @@
       <c r="B10" s="45"/>
       <c r="F10" s="111"/>
       <c r="I10" s="111"/>
-      <c r="M10" s="113"/>
-      <c r="N10" s="111"/>
-      <c r="O10" s="111"/>
-      <c r="P10" s="111"/>
+      <c r="J10" s="111"/>
+      <c r="K10" s="111"/>
+      <c r="P10" s="112"/>
+      <c r="Q10" s="111"/>
+      <c r="R10" s="111"/>
       <c r="CV10" s="44"/>
       <c r="CW10"/>
       <c r="CX10"/>
@@ -3215,17 +3222,18 @@
         <v>13</v>
       </c>
       <c r="B11" s="45"/>
-      <c r="G11" s="113" t="s">
+      <c r="G11" s="112" t="s">
         <v>81</v>
       </c>
-      <c r="H11" s="113" t="s">
+      <c r="H11" s="112" t="s">
         <v>82</v>
       </c>
       <c r="I11" s="111"/>
-      <c r="M11" s="111"/>
-      <c r="N11" s="111"/>
-      <c r="O11" s="111"/>
+      <c r="J11" s="111"/>
+      <c r="K11" s="111"/>
       <c r="P11" s="111"/>
+      <c r="Q11" s="111"/>
+      <c r="R11" s="111"/>
       <c r="CV11" s="44"/>
       <c r="CW11"/>
       <c r="CX11"/>
@@ -3293,12 +3301,11 @@
         <v>11</v>
       </c>
       <c r="B12" s="45"/>
-      <c r="G12" s="115"/>
-      <c r="H12" s="115"/>
-      <c r="M12" s="111"/>
-      <c r="N12" s="111"/>
-      <c r="O12" s="111"/>
+      <c r="G12" s="114"/>
+      <c r="H12" s="114"/>
       <c r="P12" s="111"/>
+      <c r="Q12" s="111"/>
+      <c r="R12" s="111"/>
       <c r="CV12" s="44"/>
       <c r="CW12"/>
       <c r="CX12"/>
@@ -3366,16 +3373,18 @@
         <v>9</v>
       </c>
       <c r="B13" s="45"/>
-      <c r="J13" s="113" t="s">
+      <c r="L13" s="112" t="s">
         <v>90</v>
       </c>
-      <c r="K13" s="113" t="s">
+      <c r="M13" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="N13" s="112" t="s">
         <v>91</v>
       </c>
-      <c r="M13" s="111"/>
-      <c r="N13" s="111"/>
-      <c r="O13" s="111"/>
       <c r="P13" s="111"/>
+      <c r="Q13" s="111"/>
+      <c r="R13" s="111"/>
       <c r="CV13" s="44"/>
       <c r="CW13"/>
       <c r="CX13"/>
@@ -3443,12 +3452,12 @@
         <v>16</v>
       </c>
       <c r="B14" s="45"/>
-      <c r="J14" s="111"/>
-      <c r="K14" s="111"/>
+      <c r="L14" s="111"/>
       <c r="M14" s="111"/>
       <c r="N14" s="111"/>
-      <c r="O14" s="111"/>
       <c r="P14" s="111"/>
+      <c r="Q14" s="111"/>
+      <c r="R14" s="111"/>
       <c r="CV14" s="44"/>
       <c r="CW14"/>
       <c r="CX14"/>
@@ -3516,12 +3525,12 @@
         <v>14</v>
       </c>
       <c r="B15" s="45"/>
-      <c r="J15" s="111"/>
-      <c r="K15" s="111"/>
+      <c r="L15" s="111"/>
       <c r="M15" s="111"/>
       <c r="N15" s="111"/>
-      <c r="O15" s="111"/>
       <c r="P15" s="111"/>
+      <c r="Q15" s="111"/>
+      <c r="R15" s="111"/>
       <c r="CV15" s="44"/>
       <c r="CW15"/>
       <c r="CX15"/>
@@ -3589,12 +3598,12 @@
         <v>15</v>
       </c>
       <c r="B16" s="45"/>
-      <c r="J16" s="111"/>
-      <c r="K16" s="111"/>
+      <c r="L16" s="111"/>
       <c r="M16" s="111"/>
       <c r="N16" s="111"/>
-      <c r="O16" s="111"/>
       <c r="P16" s="111"/>
+      <c r="Q16" s="111"/>
+      <c r="R16" s="111"/>
       <c r="CV16" s="44"/>
       <c r="CW16"/>
       <c r="CX16"/>
@@ -3664,13 +3673,10 @@
       <c r="B17" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="N17" s="114" t="s">
+      <c r="Q17" s="113" t="s">
         <v>80</v>
       </c>
-      <c r="O17" s="114" t="s">
-        <v>80</v>
-      </c>
-      <c r="P17" s="114" t="s">
+      <c r="R17" s="113" t="s">
         <v>80</v>
       </c>
       <c r="CV17" s="47"/>
@@ -3824,37 +3830,35 @@
       <c r="N19" s="85"/>
       <c r="O19" s="85"/>
       <c r="P19" s="85"/>
-      <c r="Q19" s="122"/>
-      <c r="R19" s="122"/>
-      <c r="S19" s="122"/>
-      <c r="T19" s="85"/>
-      <c r="U19" s="85"/>
+      <c r="Q19" s="85"/>
+      <c r="R19" s="85"/>
+      <c r="S19" s="121"/>
+      <c r="T19" s="121"/>
+      <c r="U19" s="121"/>
       <c r="V19" s="85"/>
       <c r="W19" s="85"/>
       <c r="X19" s="85"/>
       <c r="Y19" s="85"/>
-      <c r="Z19" s="144"/>
+      <c r="Z19" s="143"/>
       <c r="AA19" s="85"/>
       <c r="AB19" s="85"/>
       <c r="AC19" s="85"/>
       <c r="AD19" s="85"/>
       <c r="AE19" s="85"/>
       <c r="AF19" s="85"/>
-      <c r="AG19" s="123"/>
-      <c r="AH19" s="130" t="s">
+      <c r="AG19" s="122"/>
+      <c r="AH19" s="122"/>
+      <c r="AI19" s="122"/>
+      <c r="AJ19" s="129" t="s">
         <v>79</v>
       </c>
-      <c r="AI19" s="130" t="s">
+      <c r="AK19" s="129" t="s">
         <v>79</v>
       </c>
-      <c r="AJ19" s="130" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK19" s="130"/>
-      <c r="AL19" s="130"/>
-      <c r="AM19" s="130"/>
-      <c r="AN19" s="130"/>
-      <c r="AO19" s="130"/>
+      <c r="AL19" s="129"/>
+      <c r="AM19" s="129"/>
+      <c r="AN19" s="129"/>
+      <c r="AO19" s="129"/>
       <c r="AP19" s="85"/>
       <c r="AQ19" s="85"/>
       <c r="AR19" s="85"/>
@@ -3994,16 +3998,16 @@
       <c r="N20" s="85"/>
       <c r="O20" s="85"/>
       <c r="P20" s="85"/>
-      <c r="Q20" s="122"/>
+      <c r="Q20" s="85"/>
       <c r="R20" s="85"/>
-      <c r="S20" s="85"/>
+      <c r="S20" s="121"/>
       <c r="T20" s="85"/>
       <c r="U20" s="85"/>
       <c r="V20" s="85"/>
       <c r="W20" s="85"/>
       <c r="X20" s="85"/>
       <c r="Y20" s="85"/>
-      <c r="Z20" s="144"/>
+      <c r="Z20" s="143"/>
       <c r="AA20" s="85"/>
       <c r="AB20" s="85"/>
       <c r="AC20" s="85"/>
@@ -4159,38 +4163,38 @@
       <c r="O21" s="85"/>
       <c r="P21" s="85"/>
       <c r="Q21" s="85"/>
-      <c r="R21" s="122"/>
-      <c r="S21" s="130"/>
-      <c r="T21" s="130"/>
-      <c r="U21" s="130"/>
-      <c r="V21" s="122"/>
-      <c r="W21" s="122"/>
-      <c r="X21" s="130"/>
-      <c r="Y21" s="122"/>
-      <c r="Z21" s="137" t="s">
+      <c r="R21" s="85"/>
+      <c r="S21" s="85"/>
+      <c r="T21" s="121"/>
+      <c r="U21" s="129"/>
+      <c r="V21" s="121"/>
+      <c r="W21" s="121"/>
+      <c r="X21" s="121"/>
+      <c r="Y21" s="121"/>
+      <c r="Z21" s="136"/>
+      <c r="AA21" s="136"/>
+      <c r="AB21" s="136" t="s">
         <v>94</v>
       </c>
-      <c r="AA21" s="137" t="s">
+      <c r="AC21" s="136" t="s">
         <v>94</v>
       </c>
-      <c r="AB21" s="122"/>
-      <c r="AC21" s="122"/>
-      <c r="AD21" s="122"/>
-      <c r="AE21" s="122"/>
-      <c r="AF21" s="130" t="s">
+      <c r="AD21" s="121"/>
+      <c r="AE21" s="121"/>
+      <c r="AF21" s="129"/>
+      <c r="AG21" s="129"/>
+      <c r="AH21" s="129" t="s">
         <v>83</v>
       </c>
-      <c r="AG21" s="130" t="s">
+      <c r="AI21" s="129" t="s">
         <v>83</v>
       </c>
-      <c r="AH21" s="122"/>
-      <c r="AI21" s="122"/>
-      <c r="AJ21" s="122"/>
-      <c r="AK21" s="130"/>
-      <c r="AL21" s="130"/>
-      <c r="AM21" s="130"/>
-      <c r="AN21" s="130"/>
-      <c r="AO21" s="130"/>
+      <c r="AJ21" s="121"/>
+      <c r="AK21" s="121"/>
+      <c r="AL21" s="129"/>
+      <c r="AM21" s="129"/>
+      <c r="AN21" s="129"/>
+      <c r="AO21" s="129"/>
       <c r="AP21" s="85"/>
       <c r="AQ21" s="85"/>
       <c r="AR21" s="85"/>
@@ -4332,31 +4336,33 @@
       <c r="P22" s="85"/>
       <c r="Q22" s="85"/>
       <c r="R22" s="85"/>
-      <c r="S22" s="122"/>
-      <c r="T22" s="130"/>
-      <c r="U22" s="130"/>
-      <c r="V22" s="122"/>
-      <c r="W22" s="122"/>
-      <c r="X22" s="130" t="s">
+      <c r="S22" s="85"/>
+      <c r="T22" s="85"/>
+      <c r="U22" s="121"/>
+      <c r="V22" s="121"/>
+      <c r="W22" s="121"/>
+      <c r="X22" s="121"/>
+      <c r="Y22" s="121"/>
+      <c r="Z22" s="129" t="s">
         <v>58</v>
       </c>
-      <c r="Y22" s="122"/>
-      <c r="Z22" s="134"/>
-      <c r="AA22" s="122"/>
-      <c r="AB22" s="122"/>
-      <c r="AC22" s="122"/>
-      <c r="AD22" s="122"/>
-      <c r="AE22" s="122"/>
-      <c r="AF22" s="122"/>
-      <c r="AG22" s="122"/>
-      <c r="AH22" s="122"/>
-      <c r="AI22" s="122"/>
-      <c r="AJ22" s="122"/>
-      <c r="AK22" s="130"/>
-      <c r="AL22" s="130"/>
-      <c r="AM22" s="130"/>
-      <c r="AN22" s="130"/>
-      <c r="AO22" s="130"/>
+      <c r="AA22" s="129" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB22" s="121"/>
+      <c r="AC22" s="121"/>
+      <c r="AD22" s="121"/>
+      <c r="AE22" s="121"/>
+      <c r="AF22" s="121"/>
+      <c r="AG22" s="121"/>
+      <c r="AH22" s="121"/>
+      <c r="AI22" s="121"/>
+      <c r="AJ22" s="121"/>
+      <c r="AK22" s="121"/>
+      <c r="AL22" s="129"/>
+      <c r="AM22" s="129"/>
+      <c r="AN22" s="129"/>
+      <c r="AO22" s="129"/>
       <c r="AP22" s="85"/>
       <c r="AQ22" s="85"/>
       <c r="AR22" s="85"/>
@@ -4498,33 +4504,33 @@
       <c r="P23" s="85"/>
       <c r="Q23" s="85"/>
       <c r="R23" s="85"/>
-      <c r="S23" s="130" t="s">
+      <c r="S23" s="85"/>
+      <c r="T23" s="85"/>
+      <c r="U23" s="129" t="s">
         <v>92</v>
       </c>
-      <c r="T23" s="130"/>
-      <c r="U23" s="130"/>
-      <c r="V23" s="122"/>
-      <c r="W23" s="122"/>
-      <c r="X23" s="122"/>
-      <c r="Y23" s="122"/>
-      <c r="Z23" s="134"/>
-      <c r="AA23" s="122"/>
-      <c r="AB23" s="130" t="s">
+      <c r="V23" s="121"/>
+      <c r="W23" s="121"/>
+      <c r="X23" s="121"/>
+      <c r="Y23" s="121"/>
+      <c r="Z23" s="133"/>
+      <c r="AA23" s="121"/>
+      <c r="AB23" s="121"/>
+      <c r="AC23" s="121"/>
+      <c r="AD23" s="129" t="s">
         <v>93</v>
       </c>
-      <c r="AC23" s="122"/>
-      <c r="AD23" s="122"/>
-      <c r="AE23" s="122"/>
-      <c r="AF23" s="122"/>
-      <c r="AG23" s="122"/>
-      <c r="AH23" s="122"/>
-      <c r="AI23" s="122"/>
-      <c r="AJ23" s="122"/>
-      <c r="AK23" s="130"/>
-      <c r="AL23" s="130"/>
-      <c r="AM23" s="130"/>
-      <c r="AN23" s="130"/>
-      <c r="AO23" s="130"/>
+      <c r="AE23" s="121"/>
+      <c r="AF23" s="121"/>
+      <c r="AG23" s="121"/>
+      <c r="AH23" s="121"/>
+      <c r="AI23" s="121"/>
+      <c r="AJ23" s="121"/>
+      <c r="AK23" s="121"/>
+      <c r="AL23" s="129"/>
+      <c r="AM23" s="129"/>
+      <c r="AN23" s="129"/>
+      <c r="AO23" s="129"/>
       <c r="AP23" s="85"/>
       <c r="AQ23" s="85"/>
       <c r="AR23" s="85"/>
@@ -4665,30 +4671,30 @@
       <c r="O24" s="85"/>
       <c r="P24" s="85"/>
       <c r="Q24" s="85"/>
-      <c r="R24" s="123"/>
-      <c r="S24" s="123"/>
-      <c r="T24" s="130"/>
-      <c r="U24" s="130"/>
-      <c r="V24" s="134"/>
-      <c r="W24" s="134"/>
-      <c r="X24" s="122"/>
-      <c r="Y24" s="134"/>
-      <c r="Z24" s="134"/>
-      <c r="AA24" s="122"/>
-      <c r="AB24" s="122"/>
-      <c r="AC24" s="122"/>
-      <c r="AD24" s="122"/>
-      <c r="AE24" s="122"/>
-      <c r="AF24" s="122"/>
-      <c r="AG24" s="122"/>
-      <c r="AH24" s="122"/>
-      <c r="AI24" s="122"/>
-      <c r="AJ24" s="122"/>
-      <c r="AK24" s="130"/>
-      <c r="AL24" s="130"/>
-      <c r="AM24" s="130"/>
-      <c r="AN24" s="130"/>
-      <c r="AO24" s="130"/>
+      <c r="R24" s="122"/>
+      <c r="S24" s="85"/>
+      <c r="T24" s="122"/>
+      <c r="U24" s="122"/>
+      <c r="V24" s="133"/>
+      <c r="W24" s="133"/>
+      <c r="X24" s="133"/>
+      <c r="Y24" s="133"/>
+      <c r="Z24" s="133"/>
+      <c r="AA24" s="121"/>
+      <c r="AB24" s="121"/>
+      <c r="AC24" s="121"/>
+      <c r="AD24" s="121"/>
+      <c r="AE24" s="121"/>
+      <c r="AF24" s="121"/>
+      <c r="AG24" s="121"/>
+      <c r="AH24" s="121"/>
+      <c r="AI24" s="121"/>
+      <c r="AJ24" s="121"/>
+      <c r="AK24" s="121"/>
+      <c r="AL24" s="129"/>
+      <c r="AM24" s="129"/>
+      <c r="AN24" s="129"/>
+      <c r="AO24" s="129"/>
       <c r="AP24" s="85"/>
       <c r="AQ24" s="85"/>
       <c r="AR24" s="85"/>
@@ -4831,28 +4837,28 @@
       <c r="Q25" s="85"/>
       <c r="R25" s="85"/>
       <c r="S25" s="85"/>
-      <c r="T25" s="130"/>
-      <c r="U25" s="130"/>
-      <c r="V25" s="122"/>
-      <c r="W25" s="122"/>
-      <c r="X25" s="122"/>
-      <c r="Y25" s="122"/>
-      <c r="Z25" s="134"/>
-      <c r="AA25" s="135"/>
-      <c r="AB25" s="135"/>
-      <c r="AC25" s="122"/>
-      <c r="AD25" s="136"/>
-      <c r="AE25" s="122"/>
-      <c r="AF25" s="130"/>
-      <c r="AG25" s="122"/>
-      <c r="AH25" s="122"/>
-      <c r="AI25" s="122"/>
-      <c r="AJ25" s="122"/>
-      <c r="AK25" s="130"/>
-      <c r="AL25" s="130"/>
-      <c r="AM25" s="130"/>
-      <c r="AN25" s="130"/>
-      <c r="AO25" s="130"/>
+      <c r="T25" s="85"/>
+      <c r="U25" s="85"/>
+      <c r="V25" s="121"/>
+      <c r="W25" s="121"/>
+      <c r="X25" s="121"/>
+      <c r="Y25" s="121"/>
+      <c r="Z25" s="133"/>
+      <c r="AA25" s="134"/>
+      <c r="AB25" s="134"/>
+      <c r="AC25" s="134"/>
+      <c r="AD25" s="135"/>
+      <c r="AE25" s="121"/>
+      <c r="AF25" s="129"/>
+      <c r="AG25" s="121"/>
+      <c r="AH25" s="121"/>
+      <c r="AI25" s="121"/>
+      <c r="AJ25" s="121"/>
+      <c r="AK25" s="121"/>
+      <c r="AL25" s="129"/>
+      <c r="AM25" s="129"/>
+      <c r="AN25" s="129"/>
+      <c r="AO25" s="129"/>
       <c r="AP25" s="85"/>
       <c r="AQ25" s="85"/>
       <c r="AR25" s="85"/>
@@ -4999,24 +5005,24 @@
       <c r="U26" s="85"/>
       <c r="V26" s="85"/>
       <c r="W26" s="85"/>
-      <c r="X26" s="122"/>
-      <c r="Y26" s="122"/>
-      <c r="Z26" s="134"/>
-      <c r="AA26" s="135"/>
-      <c r="AB26" s="135"/>
-      <c r="AC26" s="122"/>
-      <c r="AD26" s="136"/>
-      <c r="AE26" s="122"/>
-      <c r="AF26" s="130"/>
-      <c r="AG26" s="122"/>
-      <c r="AH26" s="122"/>
-      <c r="AI26" s="122"/>
-      <c r="AJ26" s="122"/>
-      <c r="AK26" s="130"/>
-      <c r="AL26" s="130"/>
-      <c r="AM26" s="130"/>
-      <c r="AN26" s="130"/>
-      <c r="AO26" s="130"/>
+      <c r="X26" s="85"/>
+      <c r="Y26" s="85"/>
+      <c r="Z26" s="133"/>
+      <c r="AA26" s="134"/>
+      <c r="AB26" s="134"/>
+      <c r="AC26" s="134"/>
+      <c r="AD26" s="135"/>
+      <c r="AE26" s="121"/>
+      <c r="AF26" s="129"/>
+      <c r="AG26" s="121"/>
+      <c r="AH26" s="121"/>
+      <c r="AI26" s="121"/>
+      <c r="AJ26" s="121"/>
+      <c r="AK26" s="121"/>
+      <c r="AL26" s="129"/>
+      <c r="AM26" s="129"/>
+      <c r="AN26" s="129"/>
+      <c r="AO26" s="129"/>
       <c r="AP26" s="85"/>
       <c r="AQ26" s="85"/>
       <c r="AR26" s="85"/>
@@ -5158,29 +5164,29 @@
       <c r="P27" s="85"/>
       <c r="Q27" s="85"/>
       <c r="R27" s="85"/>
-      <c r="S27" s="122"/>
-      <c r="T27" s="122"/>
-      <c r="U27" s="122"/>
-      <c r="V27" s="122"/>
-      <c r="W27" s="122"/>
-      <c r="X27" s="122"/>
-      <c r="Y27" s="122"/>
-      <c r="Z27" s="134"/>
-      <c r="AA27" s="122"/>
-      <c r="AB27" s="122"/>
-      <c r="AC27" s="122"/>
-      <c r="AD27" s="122"/>
-      <c r="AE27" s="122"/>
-      <c r="AF27" s="122"/>
-      <c r="AG27" s="122"/>
-      <c r="AH27" s="122"/>
-      <c r="AI27" s="122"/>
-      <c r="AJ27" s="122"/>
-      <c r="AK27" s="130"/>
-      <c r="AL27" s="130"/>
-      <c r="AM27" s="130"/>
-      <c r="AN27" s="130"/>
-      <c r="AO27" s="130"/>
+      <c r="S27" s="85"/>
+      <c r="T27" s="85"/>
+      <c r="U27" s="121"/>
+      <c r="V27" s="121"/>
+      <c r="W27" s="121"/>
+      <c r="X27" s="121"/>
+      <c r="Y27" s="121"/>
+      <c r="Z27" s="133"/>
+      <c r="AA27" s="121"/>
+      <c r="AB27" s="121"/>
+      <c r="AC27" s="121"/>
+      <c r="AD27" s="121"/>
+      <c r="AE27" s="121"/>
+      <c r="AF27" s="121"/>
+      <c r="AG27" s="121"/>
+      <c r="AH27" s="121"/>
+      <c r="AI27" s="121"/>
+      <c r="AJ27" s="121"/>
+      <c r="AK27" s="121"/>
+      <c r="AL27" s="129"/>
+      <c r="AM27" s="129"/>
+      <c r="AN27" s="129"/>
+      <c r="AO27" s="129"/>
       <c r="AP27" s="85"/>
       <c r="AQ27" s="85"/>
       <c r="AR27" s="85"/>
@@ -5329,7 +5335,7 @@
       <c r="W28" s="85"/>
       <c r="X28" s="85"/>
       <c r="Y28" s="85"/>
-      <c r="Z28" s="144"/>
+      <c r="Z28" s="143"/>
       <c r="AA28" s="85"/>
       <c r="AB28" s="85"/>
       <c r="AC28" s="85"/>
@@ -5337,14 +5343,14 @@
       <c r="AE28" s="85"/>
       <c r="AF28" s="85"/>
       <c r="AG28" s="85"/>
-      <c r="AH28" s="122"/>
-      <c r="AI28" s="122"/>
-      <c r="AJ28" s="122"/>
-      <c r="AK28" s="130"/>
-      <c r="AL28" s="130"/>
-      <c r="AM28" s="130"/>
-      <c r="AN28" s="130"/>
-      <c r="AO28" s="130"/>
+      <c r="AH28" s="85"/>
+      <c r="AI28" s="85"/>
+      <c r="AJ28" s="121"/>
+      <c r="AK28" s="121"/>
+      <c r="AL28" s="129"/>
+      <c r="AM28" s="129"/>
+      <c r="AN28" s="129"/>
+      <c r="AO28" s="129"/>
       <c r="AP28" s="85"/>
       <c r="AQ28" s="85"/>
       <c r="AR28" s="85"/>
@@ -5501,14 +5507,14 @@
       <c r="AE29" s="85"/>
       <c r="AF29" s="85"/>
       <c r="AG29" s="85"/>
-      <c r="AH29" s="122"/>
-      <c r="AI29" s="122"/>
-      <c r="AJ29" s="122"/>
-      <c r="AK29" s="130"/>
-      <c r="AL29" s="130"/>
-      <c r="AM29" s="130"/>
-      <c r="AN29" s="130"/>
-      <c r="AO29" s="130"/>
+      <c r="AH29" s="85"/>
+      <c r="AI29" s="85"/>
+      <c r="AJ29" s="121"/>
+      <c r="AK29" s="121"/>
+      <c r="AL29" s="129"/>
+      <c r="AM29" s="129"/>
+      <c r="AN29" s="129"/>
+      <c r="AO29" s="129"/>
       <c r="AP29" s="85"/>
       <c r="AQ29" s="85"/>
       <c r="AR29" s="85"/>
@@ -5669,20 +5675,18 @@
       <c r="AG30" s="91"/>
       <c r="AH30" s="91"/>
       <c r="AI30" s="91"/>
-      <c r="AJ30" s="138"/>
-      <c r="AK30" s="126" t="s">
+      <c r="AJ30" s="137"/>
+      <c r="AK30" s="137"/>
+      <c r="AL30" s="125" t="s">
         <v>80</v>
       </c>
-      <c r="AL30" s="126" t="s">
+      <c r="AM30" s="125" t="s">
         <v>80</v>
       </c>
-      <c r="AM30" s="126" t="s">
+      <c r="AN30" s="125" t="s">
         <v>80</v>
       </c>
-      <c r="AN30" s="126" t="s">
-        <v>80</v>
-      </c>
-      <c r="AO30" s="126" t="s">
+      <c r="AO30" s="125" t="s">
         <v>80</v>
       </c>
       <c r="AP30" s="91"/>
@@ -5912,8 +5916,8 @@
       <c r="BG32" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="BH32" s="125"/>
-      <c r="BI32" s="125"/>
+      <c r="BH32" s="124"/>
+      <c r="BI32" s="124"/>
       <c r="CV32" s="51"/>
       <c r="CW32"/>
       <c r="CX32"/>
@@ -5982,8 +5986,8 @@
       </c>
       <c r="B33" s="50"/>
       <c r="AP33" s="40"/>
-      <c r="AS33" s="125"/>
-      <c r="AT33" s="125"/>
+      <c r="AS33" s="124"/>
+      <c r="AT33" s="124"/>
       <c r="AU33" s="66" t="s">
         <v>57</v>
       </c>
@@ -6001,8 +6005,8 @@
       <c r="BE33" s="66"/>
       <c r="BF33" s="66"/>
       <c r="BG33" s="66"/>
-      <c r="BH33" s="125"/>
-      <c r="BI33" s="125"/>
+      <c r="BH33" s="124"/>
+      <c r="BI33" s="124"/>
       <c r="CV33" s="51"/>
       <c r="CW33"/>
       <c r="CX33"/>
@@ -6081,8 +6085,8 @@
       <c r="BE34" s="66"/>
       <c r="BF34" s="66"/>
       <c r="BG34" s="66"/>
-      <c r="BH34" s="125"/>
-      <c r="BI34" s="125"/>
+      <c r="BH34" s="124"/>
+      <c r="BI34" s="124"/>
       <c r="CV34" s="51"/>
       <c r="CW34"/>
       <c r="CX34"/>
@@ -6162,8 +6166,8 @@
       <c r="BE35" s="66"/>
       <c r="BF35" s="66"/>
       <c r="BG35" s="66"/>
-      <c r="BH35" s="125"/>
-      <c r="BI35" s="125"/>
+      <c r="BH35" s="124"/>
+      <c r="BI35" s="124"/>
       <c r="CV35" s="51"/>
       <c r="CW35"/>
       <c r="CX35"/>
@@ -6242,8 +6246,8 @@
       <c r="BE36" s="66"/>
       <c r="BF36" s="66"/>
       <c r="BG36" s="66"/>
-      <c r="BH36" s="125"/>
-      <c r="BI36" s="125"/>
+      <c r="BH36" s="124"/>
+      <c r="BI36" s="124"/>
       <c r="CV36" s="51"/>
       <c r="CW36"/>
       <c r="CX36"/>
@@ -6325,7 +6329,7 @@
       <c r="AT37" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="BG37" s="127"/>
+      <c r="BG37" s="126"/>
       <c r="BH37" s="67" t="s">
         <v>80</v>
       </c>
@@ -6642,7 +6646,7 @@
       <c r="BL39" s="104"/>
       <c r="BM39" s="104"/>
       <c r="BN39" s="104"/>
-      <c r="BO39" s="141"/>
+      <c r="BO39" s="140"/>
       <c r="BP39" s="104"/>
       <c r="BQ39" s="104"/>
       <c r="BR39" s="104"/>
@@ -6806,7 +6810,7 @@
       <c r="BL40" s="104"/>
       <c r="BM40" s="104"/>
       <c r="BN40" s="104"/>
-      <c r="BO40" s="140"/>
+      <c r="BO40" s="139"/>
       <c r="BP40" s="104"/>
       <c r="BQ40" s="104"/>
       <c r="BR40" s="104"/>
@@ -6971,29 +6975,29 @@
       <c r="BM41" s="104"/>
       <c r="BN41" s="104"/>
       <c r="BO41" s="104"/>
-      <c r="BP41" s="140"/>
-      <c r="BQ41" s="141" t="s">
+      <c r="BP41" s="139"/>
+      <c r="BQ41" s="140" t="s">
         <v>79</v>
       </c>
-      <c r="BR41" s="141" t="s">
+      <c r="BR41" s="140" t="s">
         <v>79</v>
       </c>
-      <c r="BS41" s="141" t="s">
+      <c r="BS41" s="140" t="s">
         <v>79</v>
       </c>
-      <c r="BT41" s="141" t="s">
+      <c r="BT41" s="140" t="s">
         <v>98</v>
       </c>
-      <c r="BU41" s="141" t="s">
+      <c r="BU41" s="140" t="s">
         <v>98</v>
       </c>
-      <c r="BV41" s="141" t="s">
+      <c r="BV41" s="140" t="s">
         <v>98</v>
       </c>
-      <c r="BW41" s="141" t="s">
+      <c r="BW41" s="140" t="s">
         <v>98</v>
       </c>
-      <c r="BX41" s="141" t="s">
+      <c r="BX41" s="140" t="s">
         <v>98</v>
       </c>
       <c r="BY41" s="104"/>
@@ -7152,14 +7156,14 @@
       <c r="BN42" s="104"/>
       <c r="BO42" s="104"/>
       <c r="BP42" s="104"/>
-      <c r="BQ42" s="140"/>
-      <c r="BR42" s="140"/>
-      <c r="BS42" s="140"/>
-      <c r="BT42" s="141"/>
-      <c r="BU42" s="141"/>
-      <c r="BV42" s="141"/>
-      <c r="BW42" s="141"/>
-      <c r="BX42" s="141"/>
+      <c r="BQ42" s="139"/>
+      <c r="BR42" s="139"/>
+      <c r="BS42" s="139"/>
+      <c r="BT42" s="140"/>
+      <c r="BU42" s="140"/>
+      <c r="BV42" s="140"/>
+      <c r="BW42" s="140"/>
+      <c r="BX42" s="140"/>
       <c r="BY42" s="104"/>
       <c r="BZ42" s="104"/>
       <c r="CA42" s="104"/>
@@ -7316,14 +7320,14 @@
       <c r="BN43" s="104"/>
       <c r="BO43" s="104"/>
       <c r="BP43" s="104"/>
-      <c r="BQ43" s="140"/>
-      <c r="BR43" s="140"/>
-      <c r="BS43" s="140"/>
-      <c r="BT43" s="141"/>
-      <c r="BU43" s="141"/>
-      <c r="BV43" s="141"/>
-      <c r="BW43" s="141"/>
-      <c r="BX43" s="141"/>
+      <c r="BQ43" s="139"/>
+      <c r="BR43" s="139"/>
+      <c r="BS43" s="139"/>
+      <c r="BT43" s="140"/>
+      <c r="BU43" s="140"/>
+      <c r="BV43" s="140"/>
+      <c r="BW43" s="140"/>
+      <c r="BX43" s="140"/>
       <c r="BY43" s="104"/>
       <c r="BZ43" s="104"/>
       <c r="CA43" s="104"/>
@@ -7480,14 +7484,14 @@
       <c r="BN44" s="104"/>
       <c r="BO44" s="104"/>
       <c r="BP44" s="104"/>
-      <c r="BQ44" s="140"/>
-      <c r="BR44" s="140"/>
-      <c r="BS44" s="140"/>
-      <c r="BT44" s="141"/>
-      <c r="BU44" s="141"/>
-      <c r="BV44" s="141"/>
-      <c r="BW44" s="141"/>
-      <c r="BX44" s="141"/>
+      <c r="BQ44" s="139"/>
+      <c r="BR44" s="139"/>
+      <c r="BS44" s="139"/>
+      <c r="BT44" s="140"/>
+      <c r="BU44" s="140"/>
+      <c r="BV44" s="140"/>
+      <c r="BW44" s="140"/>
+      <c r="BX44" s="140"/>
       <c r="BY44" s="104"/>
       <c r="BZ44" s="104"/>
       <c r="CA44" s="104"/>
@@ -7644,14 +7648,14 @@
       <c r="BN45" s="104"/>
       <c r="BO45" s="104"/>
       <c r="BP45" s="104"/>
-      <c r="BQ45" s="140"/>
-      <c r="BR45" s="140"/>
-      <c r="BS45" s="140"/>
-      <c r="BT45" s="141"/>
-      <c r="BU45" s="141"/>
-      <c r="BV45" s="141"/>
-      <c r="BW45" s="141"/>
-      <c r="BX45" s="141"/>
+      <c r="BQ45" s="139"/>
+      <c r="BR45" s="139"/>
+      <c r="BS45" s="139"/>
+      <c r="BT45" s="140"/>
+      <c r="BU45" s="140"/>
+      <c r="BV45" s="140"/>
+      <c r="BW45" s="140"/>
+      <c r="BX45" s="140"/>
       <c r="BY45" s="104"/>
       <c r="BZ45" s="104"/>
       <c r="CA45" s="104"/>
@@ -7818,34 +7822,34 @@
       <c r="BV46" s="99"/>
       <c r="BW46" s="100"/>
       <c r="BX46" s="99"/>
-      <c r="BY46" s="139" t="s">
+      <c r="BY46" s="138" t="s">
         <v>80</v>
       </c>
-      <c r="BZ46" s="139" t="s">
+      <c r="BZ46" s="138" t="s">
         <v>80</v>
       </c>
-      <c r="CA46" s="131" t="s">
+      <c r="CA46" s="130" t="s">
         <v>80</v>
       </c>
-      <c r="CB46" s="132" t="s">
+      <c r="CB46" s="131" t="s">
         <v>80</v>
       </c>
-      <c r="CC46" s="132" t="s">
+      <c r="CC46" s="131" t="s">
         <v>80</v>
       </c>
-      <c r="CD46" s="132" t="s">
+      <c r="CD46" s="131" t="s">
         <v>80</v>
       </c>
-      <c r="CE46" s="132" t="s">
+      <c r="CE46" s="131" t="s">
         <v>80</v>
       </c>
-      <c r="CF46" s="132" t="s">
+      <c r="CF46" s="131" t="s">
         <v>80</v>
       </c>
-      <c r="CG46" s="132" t="s">
+      <c r="CG46" s="131" t="s">
         <v>80</v>
       </c>
-      <c r="CH46" s="132" t="s">
+      <c r="CH46" s="131" t="s">
         <v>80</v>
       </c>
       <c r="CI46" s="99"/>
@@ -8078,17 +8082,17 @@
       <c r="CE48" s="14"/>
       <c r="CF48" s="14"/>
       <c r="CG48" s="14"/>
-      <c r="CH48" s="119"/>
-      <c r="CI48" s="142"/>
-      <c r="CJ48" s="142"/>
-      <c r="CK48" s="142"/>
-      <c r="CL48" s="143" t="s">
+      <c r="CH48" s="118"/>
+      <c r="CI48" s="141"/>
+      <c r="CJ48" s="141"/>
+      <c r="CK48" s="141"/>
+      <c r="CL48" s="142" t="s">
         <v>79</v>
       </c>
-      <c r="CM48" s="143" t="s">
+      <c r="CM48" s="142" t="s">
         <v>79</v>
       </c>
-      <c r="CN48" s="143" t="s">
+      <c r="CN48" s="142" t="s">
         <v>79</v>
       </c>
       <c r="CO48" s="14"/>
@@ -8249,9 +8253,9 @@
       <c r="CF49" s="14"/>
       <c r="CG49" s="14"/>
       <c r="CH49" s="14"/>
-      <c r="CI49" s="119"/>
-      <c r="CJ49" s="119"/>
-      <c r="CK49" s="119"/>
+      <c r="CI49" s="118"/>
+      <c r="CJ49" s="118"/>
+      <c r="CK49" s="118"/>
       <c r="CL49" s="14"/>
       <c r="CM49" s="14"/>
       <c r="CN49" s="14"/>
@@ -8413,12 +8417,12 @@
       <c r="CF50" s="14"/>
       <c r="CG50" s="14"/>
       <c r="CH50" s="14"/>
-      <c r="CI50" s="119"/>
-      <c r="CJ50" s="119"/>
-      <c r="CK50" s="119"/>
-      <c r="CL50" s="143"/>
-      <c r="CM50" s="143"/>
-      <c r="CN50" s="143"/>
+      <c r="CI50" s="118"/>
+      <c r="CJ50" s="118"/>
+      <c r="CK50" s="118"/>
+      <c r="CL50" s="142"/>
+      <c r="CM50" s="142"/>
+      <c r="CN50" s="142"/>
       <c r="CO50" s="14"/>
       <c r="CP50" s="14"/>
       <c r="CQ50" s="14"/>
@@ -8577,9 +8581,9 @@
       <c r="CF51" s="14"/>
       <c r="CG51" s="14"/>
       <c r="CH51" s="14"/>
-      <c r="CI51" s="119"/>
-      <c r="CJ51" s="119"/>
-      <c r="CK51" s="119"/>
+      <c r="CI51" s="118"/>
+      <c r="CJ51" s="118"/>
+      <c r="CK51" s="118"/>
       <c r="CL51" s="14"/>
       <c r="CM51" s="14"/>
       <c r="CN51" s="14"/>
@@ -8741,12 +8745,12 @@
       <c r="CF52" s="14"/>
       <c r="CG52" s="14"/>
       <c r="CH52" s="14"/>
-      <c r="CI52" s="119"/>
-      <c r="CJ52" s="119"/>
-      <c r="CK52" s="119"/>
-      <c r="CL52" s="143"/>
-      <c r="CM52" s="143"/>
-      <c r="CN52" s="143"/>
+      <c r="CI52" s="118"/>
+      <c r="CJ52" s="118"/>
+      <c r="CK52" s="118"/>
+      <c r="CL52" s="142"/>
+      <c r="CM52" s="142"/>
+      <c r="CN52" s="142"/>
       <c r="CO52" s="14"/>
       <c r="CP52" s="14"/>
       <c r="CQ52" s="14"/>
@@ -8910,29 +8914,29 @@
       <c r="CI53" s="34"/>
       <c r="CJ53" s="34"/>
       <c r="CK53" s="34"/>
-      <c r="CL53" s="133"/>
-      <c r="CM53" s="133"/>
-      <c r="CN53" s="133"/>
-      <c r="CO53" s="128" t="s">
+      <c r="CL53" s="132"/>
+      <c r="CM53" s="132"/>
+      <c r="CN53" s="132"/>
+      <c r="CO53" s="127" t="s">
         <v>80</v>
       </c>
-      <c r="CP53" s="128" t="s">
+      <c r="CP53" s="127" t="s">
         <v>80</v>
       </c>
-      <c r="CQ53" s="128" t="s">
+      <c r="CQ53" s="127" t="s">
         <v>80</v>
       </c>
-      <c r="CR53" s="128" t="s">
+      <c r="CR53" s="127" t="s">
         <v>80</v>
       </c>
-      <c r="CS53" s="128" t="s">
+      <c r="CS53" s="127" t="s">
         <v>80</v>
       </c>
-      <c r="CT53" s="128" t="s">
+      <c r="CT53" s="127" t="s">
         <v>86</v>
       </c>
-      <c r="CU53" s="128"/>
-      <c r="CV53" s="129"/>
+      <c r="CU53" s="127"/>
+      <c r="CV53" s="128"/>
       <c r="CW53"/>
       <c r="CX53"/>
       <c r="CY53"/>
@@ -9138,13 +9142,12 @@
     </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="CI1:CV1"/>
-    <mergeCell ref="B1:P1"/>
-    <mergeCell ref="Q1:AO1"/>
     <mergeCell ref="BO1:CH1"/>
     <mergeCell ref="AP1:AS1"/>
     <mergeCell ref="AT1:BN1"/>
+    <mergeCell ref="B1:R1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>